<commit_message>
sincronizacion matutina detalles con las fracciones
</commit_message>
<xml_diff>
--- a/VenusDoors/Content/img/Template.xlsx
+++ b/VenusDoors/Content/img/Template.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="41">
   <si>
     <t>DoorStyle</t>
   </si>
@@ -106,16 +106,25 @@
     <t>Overlay</t>
   </si>
   <si>
-    <t>Flat Panel</t>
-  </si>
-  <si>
-    <t>Maple</t>
-  </si>
-  <si>
-    <t>Door</t>
-  </si>
-  <si>
-    <t>Insert Door Type</t>
+    <t>WidthDecimal</t>
+  </si>
+  <si>
+    <t>HeightDecimal</t>
+  </si>
+  <si>
+    <t>Red Oak</t>
+  </si>
+  <si>
+    <t>Drawer</t>
+  </si>
+  <si>
+    <t>Overlay Door Type</t>
+  </si>
+  <si>
+    <t>Raised Panel</t>
+  </si>
+  <si>
+    <t>Knotty Alder</t>
   </si>
   <si>
     <t>Stain Grade</t>
@@ -124,16 +133,22 @@
     <t>Cope and Stick</t>
   </si>
   <si>
-    <t>Finger Pull</t>
-  </si>
-  <si>
-    <t>Ogee</t>
+    <t>Reba</t>
   </si>
   <si>
     <t>Lazy Susan</t>
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>2 1/2.</t>
+  </si>
+  <si>
+    <t>1/8.</t>
+  </si>
+  <si>
+    <t>3/16.</t>
   </si>
 </sst>
 </file>
@@ -169,8 +184,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="13" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V24"/>
+  <dimension ref="A1:X24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,12 +516,15 @@
     <col min="13" max="13" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.7109375" style="2" customWidth="1"/>
+    <col min="17" max="17" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.42578125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -550,64 +570,70 @@
       <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>11</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>14</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>22</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>23</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2">
+        <v>30</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="1">
         <v>3</v>
       </c>
-      <c r="F2">
-        <v>3</v>
-      </c>
       <c r="G2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="H2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="I2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="K2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="L2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -618,29 +644,35 @@
       <c r="O2">
         <v>5</v>
       </c>
-      <c r="P2">
-        <v>5</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="P2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q2">
+        <v>5</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="S2" t="s">
         <v>16</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
         <v>17</v>
       </c>
-      <c r="S2" t="s">
+      <c r="U2" t="s">
         <v>18</v>
       </c>
-      <c r="T2" t="s">
-        <v>34</v>
-      </c>
-      <c r="U2" t="s">
-        <v>35</v>
-      </c>
-      <c r="V2">
+      <c r="V2" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" t="s">
+        <v>37</v>
+      </c>
+      <c r="X2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -653,7 +685,7 @@
       <c r="D3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F3" t="s">
@@ -686,29 +718,35 @@
       <c r="O3">
         <v>5</v>
       </c>
-      <c r="P3">
-        <v>5</v>
-      </c>
-      <c r="Q3" t="s">
+      <c r="P3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q3">
+        <v>5</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S3" t="s">
         <v>16</v>
       </c>
-      <c r="R3" t="s">
+      <c r="T3" t="s">
         <v>17</v>
       </c>
-      <c r="S3" t="s">
+      <c r="U3" t="s">
         <v>18</v>
       </c>
-      <c r="T3" t="s">
-        <v>19</v>
-      </c>
-      <c r="U3" t="s">
-        <v>19</v>
-      </c>
-      <c r="V3">
+      <c r="V3" t="s">
+        <v>19</v>
+      </c>
+      <c r="W3" t="s">
+        <v>19</v>
+      </c>
+      <c r="X3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -721,7 +759,7 @@
       <c r="D4" t="s">
         <v>19</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F4" t="s">
@@ -754,29 +792,35 @@
       <c r="O4">
         <v>5</v>
       </c>
-      <c r="P4">
-        <v>5</v>
-      </c>
-      <c r="Q4" t="s">
+      <c r="P4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q4">
+        <v>5</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S4" t="s">
         <v>16</v>
       </c>
-      <c r="R4" t="s">
+      <c r="T4" t="s">
         <v>17</v>
       </c>
-      <c r="S4" t="s">
+      <c r="U4" t="s">
         <v>18</v>
       </c>
-      <c r="T4" t="s">
-        <v>19</v>
-      </c>
-      <c r="U4" t="s">
-        <v>19</v>
-      </c>
-      <c r="V4">
+      <c r="V4" t="s">
+        <v>19</v>
+      </c>
+      <c r="W4" t="s">
+        <v>19</v>
+      </c>
+      <c r="X4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -789,7 +833,7 @@
       <c r="D5" t="s">
         <v>19</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F5" t="s">
@@ -822,29 +866,35 @@
       <c r="O5">
         <v>5</v>
       </c>
-      <c r="P5">
-        <v>5</v>
-      </c>
-      <c r="Q5" t="s">
+      <c r="P5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q5">
+        <v>5</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S5" t="s">
         <v>16</v>
       </c>
-      <c r="R5" t="s">
+      <c r="T5" t="s">
         <v>17</v>
       </c>
-      <c r="S5" t="s">
+      <c r="U5" t="s">
         <v>18</v>
       </c>
-      <c r="T5" t="s">
-        <v>19</v>
-      </c>
-      <c r="U5" t="s">
-        <v>19</v>
-      </c>
-      <c r="V5">
+      <c r="V5" t="s">
+        <v>19</v>
+      </c>
+      <c r="W5" t="s">
+        <v>19</v>
+      </c>
+      <c r="X5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -857,7 +907,7 @@
       <c r="D6" t="s">
         <v>19</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F6" t="s">
@@ -890,29 +940,35 @@
       <c r="O6">
         <v>5</v>
       </c>
-      <c r="P6">
-        <v>5</v>
-      </c>
-      <c r="Q6" t="s">
+      <c r="P6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q6">
+        <v>5</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S6" t="s">
         <v>16</v>
       </c>
-      <c r="R6" t="s">
+      <c r="T6" t="s">
         <v>17</v>
       </c>
-      <c r="S6" t="s">
+      <c r="U6" t="s">
         <v>18</v>
       </c>
-      <c r="T6" t="s">
-        <v>19</v>
-      </c>
-      <c r="U6" t="s">
-        <v>19</v>
-      </c>
-      <c r="V6">
+      <c r="V6" t="s">
+        <v>19</v>
+      </c>
+      <c r="W6" t="s">
+        <v>19</v>
+      </c>
+      <c r="X6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -925,7 +981,7 @@
       <c r="D7" t="s">
         <v>19</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F7" t="s">
@@ -958,29 +1014,35 @@
       <c r="O7">
         <v>5</v>
       </c>
-      <c r="P7">
-        <v>5</v>
-      </c>
-      <c r="Q7" t="s">
+      <c r="P7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q7">
+        <v>5</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S7" t="s">
         <v>16</v>
       </c>
-      <c r="R7" t="s">
+      <c r="T7" t="s">
         <v>17</v>
       </c>
-      <c r="S7" t="s">
+      <c r="U7" t="s">
         <v>18</v>
       </c>
-      <c r="T7" t="s">
-        <v>19</v>
-      </c>
-      <c r="U7" t="s">
-        <v>19</v>
-      </c>
-      <c r="V7">
+      <c r="V7" t="s">
+        <v>19</v>
+      </c>
+      <c r="W7" t="s">
+        <v>19</v>
+      </c>
+      <c r="X7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -993,7 +1055,7 @@
       <c r="D8" t="s">
         <v>19</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F8" t="s">
@@ -1026,29 +1088,35 @@
       <c r="O8">
         <v>5</v>
       </c>
-      <c r="P8">
-        <v>5</v>
-      </c>
-      <c r="Q8" t="s">
+      <c r="P8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q8">
+        <v>5</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S8" t="s">
         <v>16</v>
       </c>
-      <c r="R8" t="s">
+      <c r="T8" t="s">
         <v>17</v>
       </c>
-      <c r="S8" t="s">
+      <c r="U8" t="s">
         <v>18</v>
       </c>
-      <c r="T8" t="s">
-        <v>19</v>
-      </c>
-      <c r="U8" t="s">
-        <v>19</v>
-      </c>
-      <c r="V8">
+      <c r="V8" t="s">
+        <v>19</v>
+      </c>
+      <c r="W8" t="s">
+        <v>19</v>
+      </c>
+      <c r="X8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1061,7 +1129,7 @@
       <c r="D9" t="s">
         <v>19</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F9" t="s">
@@ -1094,29 +1162,35 @@
       <c r="O9">
         <v>5</v>
       </c>
-      <c r="P9">
-        <v>5</v>
-      </c>
-      <c r="Q9" t="s">
+      <c r="P9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q9">
+        <v>5</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S9" t="s">
         <v>16</v>
       </c>
-      <c r="R9" t="s">
+      <c r="T9" t="s">
         <v>17</v>
       </c>
-      <c r="S9" t="s">
+      <c r="U9" t="s">
         <v>18</v>
       </c>
-      <c r="T9" t="s">
-        <v>19</v>
-      </c>
-      <c r="U9" t="s">
-        <v>19</v>
-      </c>
-      <c r="V9">
+      <c r="V9" t="s">
+        <v>19</v>
+      </c>
+      <c r="W9" t="s">
+        <v>19</v>
+      </c>
+      <c r="X9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1129,7 +1203,7 @@
       <c r="D10" t="s">
         <v>19</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F10" t="s">
@@ -1162,29 +1236,35 @@
       <c r="O10">
         <v>5</v>
       </c>
-      <c r="P10">
-        <v>5</v>
-      </c>
-      <c r="Q10" t="s">
+      <c r="P10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q10">
+        <v>5</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S10" t="s">
         <v>16</v>
       </c>
-      <c r="R10" t="s">
+      <c r="T10" t="s">
         <v>17</v>
       </c>
-      <c r="S10" t="s">
+      <c r="U10" t="s">
         <v>18</v>
       </c>
-      <c r="T10" t="s">
-        <v>19</v>
-      </c>
-      <c r="U10" t="s">
-        <v>19</v>
-      </c>
-      <c r="V10">
+      <c r="V10" t="s">
+        <v>19</v>
+      </c>
+      <c r="W10" t="s">
+        <v>19</v>
+      </c>
+      <c r="X10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1197,7 +1277,7 @@
       <c r="D11" t="s">
         <v>19</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F11" t="s">
@@ -1230,29 +1310,35 @@
       <c r="O11">
         <v>5</v>
       </c>
-      <c r="P11">
-        <v>5</v>
-      </c>
-      <c r="Q11" t="s">
+      <c r="P11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q11">
+        <v>5</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S11" t="s">
         <v>16</v>
       </c>
-      <c r="R11" t="s">
+      <c r="T11" t="s">
         <v>17</v>
       </c>
-      <c r="S11" t="s">
+      <c r="U11" t="s">
         <v>18</v>
       </c>
-      <c r="T11" t="s">
-        <v>19</v>
-      </c>
-      <c r="U11" t="s">
-        <v>19</v>
-      </c>
-      <c r="V11">
+      <c r="V11" t="s">
+        <v>19</v>
+      </c>
+      <c r="W11" t="s">
+        <v>19</v>
+      </c>
+      <c r="X11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1265,7 +1351,7 @@
       <c r="D12" t="s">
         <v>19</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F12" t="s">
@@ -1298,29 +1384,35 @@
       <c r="O12">
         <v>5</v>
       </c>
-      <c r="P12">
-        <v>5</v>
-      </c>
-      <c r="Q12" t="s">
+      <c r="P12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q12">
+        <v>5</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S12" t="s">
         <v>16</v>
       </c>
-      <c r="R12" t="s">
+      <c r="T12" t="s">
         <v>17</v>
       </c>
-      <c r="S12" t="s">
+      <c r="U12" t="s">
         <v>18</v>
       </c>
-      <c r="T12" t="s">
-        <v>19</v>
-      </c>
-      <c r="U12" t="s">
-        <v>19</v>
-      </c>
-      <c r="V12">
+      <c r="V12" t="s">
+        <v>19</v>
+      </c>
+      <c r="W12" t="s">
+        <v>19</v>
+      </c>
+      <c r="X12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1333,7 +1425,7 @@
       <c r="D13" t="s">
         <v>19</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F13" t="s">
@@ -1366,29 +1458,35 @@
       <c r="O13">
         <v>5</v>
       </c>
-      <c r="P13">
-        <v>5</v>
-      </c>
-      <c r="Q13" t="s">
+      <c r="P13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q13">
+        <v>5</v>
+      </c>
+      <c r="R13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S13" t="s">
         <v>16</v>
       </c>
-      <c r="R13" t="s">
+      <c r="T13" t="s">
         <v>17</v>
       </c>
-      <c r="S13" t="s">
+      <c r="U13" t="s">
         <v>18</v>
       </c>
-      <c r="T13" t="s">
-        <v>19</v>
-      </c>
-      <c r="U13" t="s">
-        <v>19</v>
-      </c>
-      <c r="V13">
+      <c r="V13" t="s">
+        <v>19</v>
+      </c>
+      <c r="W13" t="s">
+        <v>19</v>
+      </c>
+      <c r="X13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -1401,7 +1499,7 @@
       <c r="D14" t="s">
         <v>19</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F14" t="s">
@@ -1434,29 +1532,35 @@
       <c r="O14">
         <v>5</v>
       </c>
-      <c r="P14">
-        <v>5</v>
-      </c>
-      <c r="Q14" t="s">
+      <c r="P14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q14">
+        <v>5</v>
+      </c>
+      <c r="R14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S14" t="s">
         <v>16</v>
       </c>
-      <c r="R14" t="s">
+      <c r="T14" t="s">
         <v>17</v>
       </c>
-      <c r="S14" t="s">
+      <c r="U14" t="s">
         <v>18</v>
       </c>
-      <c r="T14" t="s">
-        <v>19</v>
-      </c>
-      <c r="U14" t="s">
-        <v>19</v>
-      </c>
-      <c r="V14">
+      <c r="V14" t="s">
+        <v>19</v>
+      </c>
+      <c r="W14" t="s">
+        <v>19</v>
+      </c>
+      <c r="X14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1469,7 +1573,7 @@
       <c r="D15" t="s">
         <v>19</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F15" t="s">
@@ -1502,29 +1606,35 @@
       <c r="O15">
         <v>5</v>
       </c>
-      <c r="P15">
-        <v>5</v>
-      </c>
-      <c r="Q15" t="s">
+      <c r="P15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q15">
+        <v>5</v>
+      </c>
+      <c r="R15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S15" t="s">
         <v>16</v>
       </c>
-      <c r="R15" t="s">
+      <c r="T15" t="s">
         <v>17</v>
       </c>
-      <c r="S15" t="s">
+      <c r="U15" t="s">
         <v>18</v>
       </c>
-      <c r="T15" t="s">
-        <v>19</v>
-      </c>
-      <c r="U15" t="s">
-        <v>19</v>
-      </c>
-      <c r="V15">
+      <c r="V15" t="s">
+        <v>19</v>
+      </c>
+      <c r="W15" t="s">
+        <v>19</v>
+      </c>
+      <c r="X15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1537,7 +1647,7 @@
       <c r="D16" t="s">
         <v>19</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F16" t="s">
@@ -1570,29 +1680,35 @@
       <c r="O16">
         <v>5</v>
       </c>
-      <c r="P16">
-        <v>5</v>
-      </c>
-      <c r="Q16" t="s">
+      <c r="P16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q16">
+        <v>5</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S16" t="s">
         <v>16</v>
       </c>
-      <c r="R16" t="s">
+      <c r="T16" t="s">
         <v>17</v>
       </c>
-      <c r="S16" t="s">
+      <c r="U16" t="s">
         <v>18</v>
       </c>
-      <c r="T16" t="s">
-        <v>19</v>
-      </c>
-      <c r="U16" t="s">
-        <v>19</v>
-      </c>
-      <c r="V16">
+      <c r="V16" t="s">
+        <v>19</v>
+      </c>
+      <c r="W16" t="s">
+        <v>19</v>
+      </c>
+      <c r="X16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1605,7 +1721,7 @@
       <c r="D17" t="s">
         <v>19</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F17" t="s">
@@ -1638,29 +1754,35 @@
       <c r="O17">
         <v>5</v>
       </c>
-      <c r="P17">
-        <v>5</v>
-      </c>
-      <c r="Q17" t="s">
+      <c r="P17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q17">
+        <v>5</v>
+      </c>
+      <c r="R17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S17" t="s">
         <v>16</v>
       </c>
-      <c r="R17" t="s">
+      <c r="T17" t="s">
         <v>17</v>
       </c>
-      <c r="S17" t="s">
+      <c r="U17" t="s">
         <v>18</v>
       </c>
-      <c r="T17" t="s">
-        <v>19</v>
-      </c>
-      <c r="U17" t="s">
-        <v>19</v>
-      </c>
-      <c r="V17">
+      <c r="V17" t="s">
+        <v>19</v>
+      </c>
+      <c r="W17" t="s">
+        <v>19</v>
+      </c>
+      <c r="X17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1673,7 +1795,7 @@
       <c r="D18" t="s">
         <v>19</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F18" t="s">
@@ -1706,29 +1828,35 @@
       <c r="O18">
         <v>5</v>
       </c>
-      <c r="P18">
-        <v>5</v>
-      </c>
-      <c r="Q18" t="s">
+      <c r="P18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q18">
+        <v>5</v>
+      </c>
+      <c r="R18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S18" t="s">
         <v>16</v>
       </c>
-      <c r="R18" t="s">
+      <c r="T18" t="s">
         <v>17</v>
       </c>
-      <c r="S18" t="s">
+      <c r="U18" t="s">
         <v>18</v>
       </c>
-      <c r="T18" t="s">
-        <v>19</v>
-      </c>
-      <c r="U18" t="s">
-        <v>19</v>
-      </c>
-      <c r="V18">
+      <c r="V18" t="s">
+        <v>19</v>
+      </c>
+      <c r="W18" t="s">
+        <v>19</v>
+      </c>
+      <c r="X18">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1741,7 +1869,7 @@
       <c r="D19" t="s">
         <v>19</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F19" t="s">
@@ -1774,29 +1902,35 @@
       <c r="O19">
         <v>5</v>
       </c>
-      <c r="P19">
-        <v>5</v>
-      </c>
-      <c r="Q19" t="s">
+      <c r="P19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q19">
+        <v>5</v>
+      </c>
+      <c r="R19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S19" t="s">
         <v>16</v>
       </c>
-      <c r="R19" t="s">
+      <c r="T19" t="s">
         <v>17</v>
       </c>
-      <c r="S19" t="s">
+      <c r="U19" t="s">
         <v>18</v>
       </c>
-      <c r="T19" t="s">
-        <v>19</v>
-      </c>
-      <c r="U19" t="s">
-        <v>19</v>
-      </c>
-      <c r="V19">
+      <c r="V19" t="s">
+        <v>19</v>
+      </c>
+      <c r="W19" t="s">
+        <v>19</v>
+      </c>
+      <c r="X19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1809,7 +1943,7 @@
       <c r="D20" t="s">
         <v>19</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F20" t="s">
@@ -1842,29 +1976,35 @@
       <c r="O20">
         <v>5</v>
       </c>
-      <c r="P20">
-        <v>5</v>
-      </c>
-      <c r="Q20" t="s">
+      <c r="P20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q20">
+        <v>5</v>
+      </c>
+      <c r="R20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S20" t="s">
         <v>16</v>
       </c>
-      <c r="R20" t="s">
+      <c r="T20" t="s">
         <v>17</v>
       </c>
-      <c r="S20" t="s">
+      <c r="U20" t="s">
         <v>18</v>
       </c>
-      <c r="T20" t="s">
-        <v>19</v>
-      </c>
-      <c r="U20" t="s">
-        <v>19</v>
-      </c>
-      <c r="V20">
+      <c r="V20" t="s">
+        <v>19</v>
+      </c>
+      <c r="W20" t="s">
+        <v>19</v>
+      </c>
+      <c r="X20">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1877,7 +2017,7 @@
       <c r="D21" t="s">
         <v>19</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F21" t="s">
@@ -1910,29 +2050,35 @@
       <c r="O21">
         <v>5</v>
       </c>
-      <c r="P21">
-        <v>5</v>
-      </c>
-      <c r="Q21" t="s">
+      <c r="P21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q21">
+        <v>5</v>
+      </c>
+      <c r="R21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S21" t="s">
         <v>16</v>
       </c>
-      <c r="R21" t="s">
+      <c r="T21" t="s">
         <v>17</v>
       </c>
-      <c r="S21" t="s">
+      <c r="U21" t="s">
         <v>18</v>
       </c>
-      <c r="T21" t="s">
-        <v>19</v>
-      </c>
-      <c r="U21" t="s">
-        <v>19</v>
-      </c>
-      <c r="V21">
+      <c r="V21" t="s">
+        <v>19</v>
+      </c>
+      <c r="W21" t="s">
+        <v>19</v>
+      </c>
+      <c r="X21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -1945,7 +2091,7 @@
       <c r="D22" t="s">
         <v>19</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F22" t="s">
@@ -1978,29 +2124,35 @@
       <c r="O22">
         <v>5</v>
       </c>
-      <c r="P22">
-        <v>5</v>
-      </c>
-      <c r="Q22" t="s">
+      <c r="P22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q22">
+        <v>5</v>
+      </c>
+      <c r="R22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S22" t="s">
         <v>16</v>
       </c>
-      <c r="R22" t="s">
+      <c r="T22" t="s">
         <v>17</v>
       </c>
-      <c r="S22" t="s">
+      <c r="U22" t="s">
         <v>18</v>
       </c>
-      <c r="T22" t="s">
-        <v>19</v>
-      </c>
-      <c r="U22" t="s">
-        <v>19</v>
-      </c>
-      <c r="V22">
+      <c r="V22" t="s">
+        <v>19</v>
+      </c>
+      <c r="W22" t="s">
+        <v>19</v>
+      </c>
+      <c r="X22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -2013,7 +2165,7 @@
       <c r="D23" t="s">
         <v>19</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F23" t="s">
@@ -2046,29 +2198,35 @@
       <c r="O23">
         <v>5</v>
       </c>
-      <c r="P23">
-        <v>5</v>
-      </c>
-      <c r="Q23" t="s">
+      <c r="P23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q23">
+        <v>5</v>
+      </c>
+      <c r="R23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S23" t="s">
         <v>16</v>
       </c>
-      <c r="R23" t="s">
+      <c r="T23" t="s">
         <v>17</v>
       </c>
-      <c r="S23" t="s">
+      <c r="U23" t="s">
         <v>18</v>
       </c>
-      <c r="T23" t="s">
-        <v>19</v>
-      </c>
-      <c r="U23" t="s">
-        <v>19</v>
-      </c>
-      <c r="V23">
+      <c r="V23" t="s">
+        <v>19</v>
+      </c>
+      <c r="W23" t="s">
+        <v>19</v>
+      </c>
+      <c r="X23">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -2081,7 +2239,7 @@
       <c r="D24" t="s">
         <v>19</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F24" t="s">
@@ -2114,45 +2272,51 @@
       <c r="O24">
         <v>5</v>
       </c>
-      <c r="P24">
-        <v>5</v>
-      </c>
-      <c r="Q24" t="s">
+      <c r="P24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q24">
+        <v>5</v>
+      </c>
+      <c r="R24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S24" t="s">
         <v>16</v>
       </c>
-      <c r="R24" t="s">
+      <c r="T24" t="s">
         <v>17</v>
       </c>
-      <c r="S24" t="s">
+      <c r="U24" t="s">
         <v>18</v>
       </c>
-      <c r="T24" t="s">
-        <v>19</v>
-      </c>
-      <c r="U24" t="s">
-        <v>19</v>
-      </c>
-      <c r="V24">
+      <c r="V24" t="s">
+        <v>19</v>
+      </c>
+      <c r="W24" t="s">
+        <v>19</v>
+      </c>
+      <c r="X24">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="19">
+  <dataValidations count="21">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O24">
       <formula1>5</formula1>
       <formula2>42</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P24">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q24">
       <formula1>5</formula1>
       <formula2>96</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U24">
       <formula1>"No Opening,Opening"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T24">
       <formula1>"Select,Right,Left"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S24">
       <formula1>"No Drill,Drill"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L24">
@@ -2179,10 +2343,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A24">
       <formula1>"Select,Flat Panel,Shaker,Reba,Small Bone,Eye Brow,Cathedral"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2:V24">
       <formula1>"Select,Lazy Susan,Single,Pair"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2:W24">
       <formula1>"Select,Yes,No"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C24">
@@ -2191,11 +2355,17 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D24">
       <formula1>"Select,Insert Door Type,Overlay Door Type"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M24 N2:N24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:N24">
       <formula1>"0,1,2,3,4"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E24 F2:F24">
-      <formula1>"Select,2.5,3"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F24">
+      <formula1>"Select,2 1/2,3"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P24 R2:R24">
+      <formula1>"Select,0/16.,1/16.,1/8.,3/16.,1/4.,5/16.,3/8.,7/16.,1/2.,9/16.,5/8.,11/16.,3/4.,13/16.,7/8.,15/16."</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2 E2:E24">
+      <formula1>"Select,2 1/2.,3"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
nuevos cambios order control y orden summary
</commit_message>
<xml_diff>
--- a/VenusDoors/Content/img/Template.xlsx
+++ b/VenusDoors/Content/img/Template.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="14">
   <si>
     <t>Width</t>
   </si>
@@ -59,6 +59,15 @@
   </si>
   <si>
     <t>Height Decimal</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>Pair</t>
+  </si>
+  <si>
+    <t>Left</t>
   </si>
 </sst>
 </file>
@@ -412,8 +421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,28 +474,28 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D2">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -500,45 +509,45 @@
         <v>5</v>
       </c>
       <c r="D3">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>5</v>
+        <v>88</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -552,45 +561,45 @@
         <v>5</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -604,45 +613,45 @@
         <v>5</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D8">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -656,45 +665,45 @@
         <v>5</v>
       </c>
       <c r="D9">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -705,7 +714,7 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D11">
         <v>5</v>
@@ -714,18 +723,18 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
@@ -734,7 +743,7 @@
         <v>5</v>
       </c>
       <c r="D12">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -746,7 +755,7 @@
         <v>0</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -757,27 +766,27 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D13">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>3</v>
@@ -786,19 +795,19 @@
         <v>5</v>
       </c>
       <c r="D14">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -809,10 +818,10 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D15">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -824,12 +833,12 @@
         <v>0</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
@@ -838,19 +847,19 @@
         <v>5</v>
       </c>
       <c r="D16">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -864,45 +873,45 @@
         <v>5</v>
       </c>
       <c r="D17">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E17">
         <v>0</v>
       </c>
       <c r="F17">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D18">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -916,45 +925,45 @@
         <v>5</v>
       </c>
       <c r="D19">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B20" t="s">
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D20">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
       <c r="F20">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="G20">
         <v>0</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>